<commit_message>
That one little space on C that ruined everything
</commit_message>
<xml_diff>
--- a/product/Sequence & Series/Sequence & Series.xlsx
+++ b/product/Sequence & Series/Sequence & Series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeahD\Desktop\treppenwitzism.github.io\product\Sequence &amp; Series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5A132D-EAA9-492B-87C5-349D58F0D49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA18E66E-7BA2-42E5-8E05-DEFC15B4F4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9F202FC3-079F-49C5-B653-3C03347390DF}"/>
+    <workbookView xWindow="-20610" yWindow="705" windowWidth="20730" windowHeight="11760" xr2:uid="{9F202FC3-079F-49C5-B653-3C03347390DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Book (2)(Sheet1)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>question</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>y = 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c </t>
   </si>
   <si>
     <t>9. Find the 10th term of the arithmetic sequence : 8, 26, 44, 62, …,</t>
@@ -988,7 +985,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1010,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1121,16 +1118,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -1161,24 +1158,24 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>170</v>
@@ -1198,10 +1195,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
       </c>
       <c r="C11">
         <v>0</v>

</xml_diff>